<commit_message>
update fluid data in elec test
</commit_message>
<xml_diff>
--- a/data_fluid/data_fluid.xlsx
+++ b/data_fluid/data_fluid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mb14g15_soton_ac_uk/Documents/_MODULES/YEAR 4/GDP/__Simulink model/_Michael/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mb14g15_soton_ac_uk/Documents/_MODULES/YEAR 4/GDP/__Simulink model/_Michael/data_fluid/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="98" documentId="8_{6312B4D1-4D33-4A6F-B8DE-66DD58A0A46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CFC680F-C662-487B-8EF3-FA09759BB686}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{AF232314-92D2-4522-964E-BF10EF534C26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{AF232314-92D2-4522-964E-BF10EF534C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Water (L) (const rho)" sheetId="1" r:id="rId1"/>
@@ -1445,9 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DEB2C8-A1F9-4C25-A940-BD97FEA7F8F1}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD42"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Create parameter, gas data files; add gas data to elec test model
</commit_message>
<xml_diff>
--- a/data_fluid/data_fluid.xlsx
+++ b/data_fluid/data_fluid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mb14g15_soton_ac_uk/Documents/_MODULES/YEAR 4/GDP/__Simulink model/_Michael/data_fluid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\_Michael\data_fluid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{6312B4D1-4D33-4A6F-B8DE-66DD58A0A46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CFC680F-C662-487B-8EF3-FA09759BB686}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26EA52A-0C5E-4144-8FB6-AA4DE5E17AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{AF232314-92D2-4522-964E-BF10EF534C26}"/>
+    <workbookView xWindow="930" yWindow="90" windowWidth="27870" windowHeight="16110" activeTab="1" xr2:uid="{AF232314-92D2-4522-964E-BF10EF534C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Water (L) (const rho)" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>Temperature (K)</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>liquid</t>
+  </si>
+  <si>
+    <t>Viscosity (uPa*s)</t>
+  </si>
+  <si>
+    <t>Therm. Cond. (mW/m*K)</t>
+  </si>
+  <si>
+    <t>Cv (kJ/kg*K)</t>
+  </si>
+  <si>
+    <t>Cp (kJ/kg*K)</t>
+  </si>
+  <si>
+    <t>Entropy (kJ/kg*K)</t>
   </si>
 </sst>
 </file>
@@ -158,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -172,7 +187,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1443,1349 +1459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DEB2C8-A1F9-4C25-A940-BD97FEA7F8F1}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>273.16000000000003</v>
-      </c>
-      <c r="B2" s="4">
-        <v>9.2437000000000005E-2</v>
-      </c>
-      <c r="C2" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2448.1999999999998</v>
-      </c>
-      <c r="F2" s="4">
-        <v>3575.5</v>
-      </c>
-      <c r="G2" s="4">
-        <v>52.506999999999998</v>
-      </c>
-      <c r="H2" s="4">
-        <v>10.071</v>
-      </c>
-      <c r="I2" s="4">
-        <v>14.196999999999999</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1261</v>
-      </c>
-      <c r="K2" s="4">
-        <v>-0.24732000000000001</v>
-      </c>
-      <c r="L2" s="5">
-        <v>8.3772E-6</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0.17344999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>278.16000000000003</v>
-      </c>
-      <c r="B3" s="4">
-        <v>9.4130000000000005E-2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2498.6999999999998</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3646.6</v>
-      </c>
-      <c r="G3" s="4">
-        <v>52.69</v>
-      </c>
-      <c r="H3" s="4">
-        <v>10.096</v>
-      </c>
-      <c r="I3" s="4">
-        <v>14.223000000000001</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1272</v>
-      </c>
-      <c r="K3" s="4">
-        <v>-0.25863999999999998</v>
-      </c>
-      <c r="L3" s="5">
-        <v>8.4829999999999999E-6</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.17598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>283.16000000000003</v>
-      </c>
-      <c r="B4" s="4">
-        <v>9.5822000000000004E-2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2549.1999999999998</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3717.8</v>
-      </c>
-      <c r="G4" s="4">
-        <v>52.87</v>
-      </c>
-      <c r="H4" s="4">
-        <v>10.119</v>
-      </c>
-      <c r="I4" s="4">
-        <v>14.246</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1283</v>
-      </c>
-      <c r="K4" s="4">
-        <v>-0.26948</v>
-      </c>
-      <c r="L4" s="5">
-        <v>8.5882000000000002E-6</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.17846999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>288.16000000000003</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.7515000000000004E-2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2599.9</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3789.1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>53.046999999999997</v>
-      </c>
-      <c r="H5" s="4">
-        <v>10.141</v>
-      </c>
-      <c r="I5" s="4">
-        <v>14.268000000000001</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1293.9000000000001</v>
-      </c>
-      <c r="K5" s="4">
-        <v>-0.27987000000000001</v>
-      </c>
-      <c r="L5" s="5">
-        <v>8.6928999999999994E-6</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.18095</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>293.16000000000003</v>
-      </c>
-      <c r="B6" s="4">
-        <v>9.9207000000000004E-2</v>
-      </c>
-      <c r="C6" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2650.6</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3860.5</v>
-      </c>
-      <c r="G6" s="4">
-        <v>53.222000000000001</v>
-      </c>
-      <c r="H6" s="4">
-        <v>10.161</v>
-      </c>
-      <c r="I6" s="4">
-        <v>14.288</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1304.7</v>
-      </c>
-      <c r="K6" s="4">
-        <v>-0.28983999999999999</v>
-      </c>
-      <c r="L6" s="5">
-        <v>8.7970000000000006E-6</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0.18339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>298.16000000000003</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.1009</v>
-      </c>
-      <c r="C7" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2701.5</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3931.9</v>
-      </c>
-      <c r="G7" s="4">
-        <v>53.393999999999998</v>
-      </c>
-      <c r="H7" s="4">
-        <v>10.18</v>
-      </c>
-      <c r="I7" s="4">
-        <v>14.305999999999999</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1315.4</v>
-      </c>
-      <c r="K7" s="4">
-        <v>-0.29942000000000002</v>
-      </c>
-      <c r="L7" s="5">
-        <v>8.9005000000000006E-6</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0.18581</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>303.16000000000003</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.10259</v>
-      </c>
-      <c r="C8" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2752.4</v>
-      </c>
-      <c r="F8" s="4">
-        <v>4003.5</v>
-      </c>
-      <c r="G8" s="4">
-        <v>53.563000000000002</v>
-      </c>
-      <c r="H8" s="4">
-        <v>10.196999999999999</v>
-      </c>
-      <c r="I8" s="4">
-        <v>14.324</v>
-      </c>
-      <c r="J8" s="4">
-        <v>1326.1</v>
-      </c>
-      <c r="K8" s="4">
-        <v>-0.30862000000000001</v>
-      </c>
-      <c r="L8" s="5">
-        <v>9.0034999999999994E-6</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0.18820999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>308.16000000000003</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.10428</v>
-      </c>
-      <c r="C9" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E9" s="4">
-        <v>2803.4</v>
-      </c>
-      <c r="F9" s="4">
-        <v>4075.2</v>
-      </c>
-      <c r="G9" s="4">
-        <v>53.73</v>
-      </c>
-      <c r="H9" s="4">
-        <v>10.212999999999999</v>
-      </c>
-      <c r="I9" s="4">
-        <v>14.339</v>
-      </c>
-      <c r="J9" s="4">
-        <v>1336.7</v>
-      </c>
-      <c r="K9" s="4">
-        <v>-0.31747999999999998</v>
-      </c>
-      <c r="L9" s="5">
-        <v>9.1060000000000006E-6</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0.19059000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>313.16000000000003</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.10598</v>
-      </c>
-      <c r="C10" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2854.5</v>
-      </c>
-      <c r="F10" s="4">
-        <v>4146.8999999999996</v>
-      </c>
-      <c r="G10" s="4">
-        <v>53.895000000000003</v>
-      </c>
-      <c r="H10" s="4">
-        <v>10.228</v>
-      </c>
-      <c r="I10" s="4">
-        <v>14.353999999999999</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1347.2</v>
-      </c>
-      <c r="K10" s="4">
-        <v>-0.32601000000000002</v>
-      </c>
-      <c r="L10" s="5">
-        <v>9.2080000000000006E-6</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0.19295000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>318.16000000000003</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.10767</v>
-      </c>
-      <c r="C11" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2905.7</v>
-      </c>
-      <c r="F11" s="4">
-        <v>4218.7</v>
-      </c>
-      <c r="G11" s="4">
-        <v>54.057000000000002</v>
-      </c>
-      <c r="H11" s="4">
-        <v>10.241</v>
-      </c>
-      <c r="I11" s="4">
-        <v>14.367000000000001</v>
-      </c>
-      <c r="J11" s="4">
-        <v>1357.6</v>
-      </c>
-      <c r="K11" s="4">
-        <v>-0.33422000000000002</v>
-      </c>
-      <c r="L11" s="5">
-        <v>9.3093999999999993E-6</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0.19528000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>323.16000000000003</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.10936</v>
-      </c>
-      <c r="C12" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D12" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2956.9</v>
-      </c>
-      <c r="F12" s="4">
-        <v>4290.6000000000004</v>
-      </c>
-      <c r="G12" s="4">
-        <v>54.216999999999999</v>
-      </c>
-      <c r="H12" s="4">
-        <v>10.254</v>
-      </c>
-      <c r="I12" s="4">
-        <v>14.38</v>
-      </c>
-      <c r="J12" s="4">
-        <v>1368</v>
-      </c>
-      <c r="K12" s="4">
-        <v>-0.34214</v>
-      </c>
-      <c r="L12" s="5">
-        <v>9.4104000000000006E-6</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0.19758999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>328.16</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.11105</v>
-      </c>
-      <c r="C13" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E13" s="4">
-        <v>3008.2</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4362.6000000000004</v>
-      </c>
-      <c r="G13" s="4">
-        <v>54.374000000000002</v>
-      </c>
-      <c r="H13" s="4">
-        <v>10.265000000000001</v>
-      </c>
-      <c r="I13" s="4">
-        <v>14.391</v>
-      </c>
-      <c r="J13" s="4">
-        <v>1378.4</v>
-      </c>
-      <c r="K13" s="4">
-        <v>-0.34977999999999998</v>
-      </c>
-      <c r="L13" s="5">
-        <v>9.5109000000000007E-6</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0.19989000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>333.16</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.11275</v>
-      </c>
-      <c r="C14" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D14" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E14" s="4">
-        <v>3059.6</v>
-      </c>
-      <c r="F14" s="4">
-        <v>4434.5</v>
-      </c>
-      <c r="G14" s="4">
-        <v>54.529000000000003</v>
-      </c>
-      <c r="H14" s="4">
-        <v>10.276</v>
-      </c>
-      <c r="I14" s="4">
-        <v>14.401999999999999</v>
-      </c>
-      <c r="J14" s="4">
-        <v>1388.6</v>
-      </c>
-      <c r="K14" s="4">
-        <v>-0.35715000000000002</v>
-      </c>
-      <c r="L14" s="5">
-        <v>9.611E-6</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0.20216999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>338.16</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.11444</v>
-      </c>
-      <c r="C15" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E15" s="4">
-        <v>3111</v>
-      </c>
-      <c r="F15" s="4">
-        <v>4506.6000000000004</v>
-      </c>
-      <c r="G15" s="4">
-        <v>54.682000000000002</v>
-      </c>
-      <c r="H15" s="4">
-        <v>10.285</v>
-      </c>
-      <c r="I15" s="4">
-        <v>14.411</v>
-      </c>
-      <c r="J15" s="4">
-        <v>1398.8</v>
-      </c>
-      <c r="K15" s="4">
-        <v>-0.36426999999999998</v>
-      </c>
-      <c r="L15" s="5">
-        <v>9.7105999999999998E-6</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0.20443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>343.16</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.11613</v>
-      </c>
-      <c r="C16" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D16" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E16" s="4">
-        <v>3162.4</v>
-      </c>
-      <c r="F16" s="4">
-        <v>4578.7</v>
-      </c>
-      <c r="G16" s="4">
-        <v>54.834000000000003</v>
-      </c>
-      <c r="H16" s="4">
-        <v>10.294</v>
-      </c>
-      <c r="I16" s="4">
-        <v>14.42</v>
-      </c>
-      <c r="J16" s="4">
-        <v>1408.9</v>
-      </c>
-      <c r="K16" s="4">
-        <v>-0.37114999999999998</v>
-      </c>
-      <c r="L16" s="5">
-        <v>9.8097000000000003E-6</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.20666999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>348.16</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.11781999999999999</v>
-      </c>
-      <c r="C17" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D17" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E17" s="4">
-        <v>3213.9</v>
-      </c>
-      <c r="F17" s="4">
-        <v>4650.8</v>
-      </c>
-      <c r="G17" s="4">
-        <v>54.981999999999999</v>
-      </c>
-      <c r="H17" s="4">
-        <v>10.302</v>
-      </c>
-      <c r="I17" s="4">
-        <v>14.428000000000001</v>
-      </c>
-      <c r="J17" s="4">
-        <v>1419</v>
-      </c>
-      <c r="K17" s="4">
-        <v>-0.37780000000000002</v>
-      </c>
-      <c r="L17" s="5">
-        <v>9.9085000000000001E-6</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0.20888999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>353.16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0.11952</v>
-      </c>
-      <c r="C18" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D18" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E18" s="4">
-        <v>3265.5</v>
-      </c>
-      <c r="F18" s="4">
-        <v>4723</v>
-      </c>
-      <c r="G18" s="4">
-        <v>55.128999999999998</v>
-      </c>
-      <c r="H18" s="4">
-        <v>10.31</v>
-      </c>
-      <c r="I18" s="4">
-        <v>14.435</v>
-      </c>
-      <c r="J18" s="4">
-        <v>1429</v>
-      </c>
-      <c r="K18" s="4">
-        <v>-0.38423000000000002</v>
-      </c>
-      <c r="L18" s="5">
-        <v>1.0006999999999999E-5</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0.21110000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>358.16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0.12121</v>
-      </c>
-      <c r="C19" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D19" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E19" s="4">
-        <v>3317</v>
-      </c>
-      <c r="F19" s="4">
-        <v>4795.2</v>
-      </c>
-      <c r="G19" s="4">
-        <v>55.274000000000001</v>
-      </c>
-      <c r="H19" s="4">
-        <v>10.316000000000001</v>
-      </c>
-      <c r="I19" s="4">
-        <v>14.442</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1439</v>
-      </c>
-      <c r="K19" s="4">
-        <v>-0.39045000000000002</v>
-      </c>
-      <c r="L19" s="5">
-        <v>1.0105000000000001E-5</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0.21329999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>363.16</v>
-      </c>
-      <c r="B20" s="4">
-        <v>0.1229</v>
-      </c>
-      <c r="C20" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D20" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E20" s="4">
-        <v>3368.6</v>
-      </c>
-      <c r="F20" s="4">
-        <v>4867.3999999999996</v>
-      </c>
-      <c r="G20" s="4">
-        <v>55.417000000000002</v>
-      </c>
-      <c r="H20" s="4">
-        <v>10.323</v>
-      </c>
-      <c r="I20" s="4">
-        <v>14.448</v>
-      </c>
-      <c r="J20" s="4">
-        <v>1448.9</v>
-      </c>
-      <c r="K20" s="4">
-        <v>-0.39648</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1.0202E-5</v>
-      </c>
-      <c r="M20" s="4">
-        <v>0.21548</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>368.16</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0.12459000000000001</v>
-      </c>
-      <c r="C21" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D21" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E21" s="4">
-        <v>3420.3</v>
-      </c>
-      <c r="F21" s="4">
-        <v>4939.7</v>
-      </c>
-      <c r="G21" s="4">
-        <v>55.558999999999997</v>
-      </c>
-      <c r="H21" s="4">
-        <v>10.327999999999999</v>
-      </c>
-      <c r="I21" s="4">
-        <v>14.454000000000001</v>
-      </c>
-      <c r="J21" s="4">
-        <v>1458.7</v>
-      </c>
-      <c r="K21" s="4">
-        <v>-0.40231</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1.0299000000000001E-5</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0.21764</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>373.16</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.12629000000000001</v>
-      </c>
-      <c r="C22" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D22" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3471.9</v>
-      </c>
-      <c r="F22" s="4">
-        <v>5012</v>
-      </c>
-      <c r="G22" s="4">
-        <v>55.698</v>
-      </c>
-      <c r="H22" s="4">
-        <v>10.333</v>
-      </c>
-      <c r="I22" s="4">
-        <v>14.459</v>
-      </c>
-      <c r="J22" s="4">
-        <v>1468.4</v>
-      </c>
-      <c r="K22" s="4">
-        <v>-0.40795999999999999</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1.0396E-5</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0.2198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>378.16</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0.12798000000000001</v>
-      </c>
-      <c r="C23" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D23" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E23" s="4">
-        <v>3523.6</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5084.3</v>
-      </c>
-      <c r="G23" s="4">
-        <v>55.835999999999999</v>
-      </c>
-      <c r="H23" s="4">
-        <v>10.337999999999999</v>
-      </c>
-      <c r="I23" s="4">
-        <v>14.464</v>
-      </c>
-      <c r="J23" s="4">
-        <v>1478.2</v>
-      </c>
-      <c r="K23" s="4">
-        <v>-0.41343999999999997</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1.0492000000000001E-5</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.22192999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>383.16</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.12967000000000001</v>
-      </c>
-      <c r="C24" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D24" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E24" s="4">
-        <v>3575.3</v>
-      </c>
-      <c r="F24" s="4">
-        <v>5156.6000000000004</v>
-      </c>
-      <c r="G24" s="4">
-        <v>55.970999999999997</v>
-      </c>
-      <c r="H24" s="4">
-        <v>10.342000000000001</v>
-      </c>
-      <c r="I24" s="4">
-        <v>14.468</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1487.8</v>
-      </c>
-      <c r="K24" s="4">
-        <v>-0.41874</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1.0587999999999999E-5</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.22406000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>388.16</v>
-      </c>
-      <c r="B25" s="4">
-        <v>0.13136</v>
-      </c>
-      <c r="C25" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D25" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E25" s="4">
-        <v>3627</v>
-      </c>
-      <c r="F25" s="4">
-        <v>5229</v>
-      </c>
-      <c r="G25" s="4">
-        <v>56.106000000000002</v>
-      </c>
-      <c r="H25" s="4">
-        <v>10.346</v>
-      </c>
-      <c r="I25" s="4">
-        <v>14.472</v>
-      </c>
-      <c r="J25" s="4">
-        <v>1497.4</v>
-      </c>
-      <c r="K25" s="4">
-        <v>-0.42388999999999999</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1.0684E-5</v>
-      </c>
-      <c r="M25" s="4">
-        <v>0.22617000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>393.16</v>
-      </c>
-      <c r="B26" s="4">
-        <v>0.13306000000000001</v>
-      </c>
-      <c r="C26" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D26" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E26" s="4">
-        <v>3678.7</v>
-      </c>
-      <c r="F26" s="4">
-        <v>5301.4</v>
-      </c>
-      <c r="G26" s="4">
-        <v>56.238</v>
-      </c>
-      <c r="H26" s="4">
-        <v>10.35</v>
-      </c>
-      <c r="I26" s="4">
-        <v>14.475</v>
-      </c>
-      <c r="J26" s="4">
-        <v>1506.9</v>
-      </c>
-      <c r="K26" s="4">
-        <v>-0.42887999999999998</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1.0779E-5</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0.22828000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>398.16</v>
-      </c>
-      <c r="B27" s="4">
-        <v>0.13475000000000001</v>
-      </c>
-      <c r="C27" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D27" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E27" s="4">
-        <v>3730.5</v>
-      </c>
-      <c r="F27" s="4">
-        <v>5373.8</v>
-      </c>
-      <c r="G27" s="4">
-        <v>56.369</v>
-      </c>
-      <c r="H27" s="4">
-        <v>10.353</v>
-      </c>
-      <c r="I27" s="4">
-        <v>14.478999999999999</v>
-      </c>
-      <c r="J27" s="4">
-        <v>1516.4</v>
-      </c>
-      <c r="K27" s="4">
-        <v>-0.43371999999999999</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1.0874E-5</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.23036999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>403.16</v>
-      </c>
-      <c r="B28" s="4">
-        <v>0.13644000000000001</v>
-      </c>
-      <c r="C28" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D28" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E28" s="4">
-        <v>3782.3</v>
-      </c>
-      <c r="F28" s="4">
-        <v>5446.2</v>
-      </c>
-      <c r="G28" s="4">
-        <v>56.497999999999998</v>
-      </c>
-      <c r="H28" s="4">
-        <v>10.356</v>
-      </c>
-      <c r="I28" s="4">
-        <v>14.481999999999999</v>
-      </c>
-      <c r="J28" s="4">
-        <v>1525.9</v>
-      </c>
-      <c r="K28" s="4">
-        <v>-0.43841999999999998</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1.0968000000000001E-5</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0.23244999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>408.16</v>
-      </c>
-      <c r="B29" s="4">
-        <v>0.13813</v>
-      </c>
-      <c r="C29" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D29" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E29" s="4">
-        <v>3834.1</v>
-      </c>
-      <c r="F29" s="4">
-        <v>5518.6</v>
-      </c>
-      <c r="G29" s="4">
-        <v>56.625999999999998</v>
-      </c>
-      <c r="H29" s="4">
-        <v>10.359</v>
-      </c>
-      <c r="I29" s="4">
-        <v>14.484</v>
-      </c>
-      <c r="J29" s="4">
-        <v>1535.2</v>
-      </c>
-      <c r="K29" s="4">
-        <v>-0.44297999999999998</v>
-      </c>
-      <c r="L29" s="5">
-        <v>1.1063000000000001E-5</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0.23452000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>413.16</v>
-      </c>
-      <c r="B30" s="4">
-        <v>0.13982</v>
-      </c>
-      <c r="C30" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D30" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E30" s="4">
-        <v>3885.9</v>
-      </c>
-      <c r="F30" s="4">
-        <v>5591</v>
-      </c>
-      <c r="G30" s="4">
-        <v>56.752000000000002</v>
-      </c>
-      <c r="H30" s="4">
-        <v>10.361000000000001</v>
-      </c>
-      <c r="I30" s="4">
-        <v>14.487</v>
-      </c>
-      <c r="J30" s="4">
-        <v>1544.6</v>
-      </c>
-      <c r="K30" s="4">
-        <v>-0.44740999999999997</v>
-      </c>
-      <c r="L30" s="5">
-        <v>1.1156E-5</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0.23658000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>418.16</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0.14152000000000001</v>
-      </c>
-      <c r="C31" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D31" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E31" s="4">
-        <v>3937.7</v>
-      </c>
-      <c r="F31" s="4">
-        <v>5663.5</v>
-      </c>
-      <c r="G31" s="4">
-        <v>56.875999999999998</v>
-      </c>
-      <c r="H31" s="4">
-        <v>10.364000000000001</v>
-      </c>
-      <c r="I31" s="4">
-        <v>14.489000000000001</v>
-      </c>
-      <c r="J31" s="4">
-        <v>1553.8</v>
-      </c>
-      <c r="K31" s="4">
-        <v>-0.45171</v>
-      </c>
-      <c r="L31" s="5">
-        <v>1.1250000000000001E-5</v>
-      </c>
-      <c r="M31" s="4">
-        <v>0.23863000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>423.16</v>
-      </c>
-      <c r="B32" s="4">
-        <v>0.14321</v>
-      </c>
-      <c r="C32" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D32" s="4">
-        <v>12.195</v>
-      </c>
-      <c r="E32" s="4">
-        <v>3989.5</v>
-      </c>
-      <c r="F32" s="4">
-        <v>5736</v>
-      </c>
-      <c r="G32" s="4">
-        <v>57</v>
-      </c>
-      <c r="H32" s="4">
-        <v>10.366</v>
-      </c>
-      <c r="I32" s="4">
-        <v>14.491</v>
-      </c>
-      <c r="J32" s="4">
-        <v>1563</v>
-      </c>
-      <c r="K32" s="4">
-        <v>-0.45589000000000002</v>
-      </c>
-      <c r="L32" s="5">
-        <v>1.1343E-5</v>
-      </c>
-      <c r="M32" s="4">
-        <v>0.24067</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23CE22A-8B52-4E0E-9B7A-5878CC3A4604}">
-  <dimension ref="A1:M32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,7 +1480,7 @@
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2823,13 +1500,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -2838,17 +1515,1389 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>273.16000000000003</v>
       </c>
       <c r="B2" s="4">
+        <v>9.2437000000000005E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2448.1999999999998</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3575.5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>52.506999999999998</v>
+      </c>
+      <c r="H2" s="4">
+        <v>10.071</v>
+      </c>
+      <c r="I2" s="4">
+        <v>14.196999999999999</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1261</v>
+      </c>
+      <c r="K2" s="4">
+        <v>-0.24732000000000001</v>
+      </c>
+      <c r="L2" s="6">
+        <v>8.3772000000000002</v>
+      </c>
+      <c r="M2" s="4">
+        <v>173.45</v>
+      </c>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>278.16000000000003</v>
+      </c>
+      <c r="B3" s="4">
+        <v>9.4130000000000005E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2498.6999999999998</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3646.6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>52.69</v>
+      </c>
+      <c r="H3" s="4">
+        <v>10.096</v>
+      </c>
+      <c r="I3" s="4">
+        <v>14.223000000000001</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1272</v>
+      </c>
+      <c r="K3" s="4">
+        <v>-0.25863999999999998</v>
+      </c>
+      <c r="L3" s="6">
+        <v>8.4830000000000005</v>
+      </c>
+      <c r="M3" s="4">
+        <v>175.98</v>
+      </c>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>283.16000000000003</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9.5822000000000004E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2549.1999999999998</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3717.8</v>
+      </c>
+      <c r="G4" s="4">
+        <v>52.87</v>
+      </c>
+      <c r="H4" s="4">
+        <v>10.119</v>
+      </c>
+      <c r="I4" s="4">
+        <v>14.246</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1283</v>
+      </c>
+      <c r="K4" s="4">
+        <v>-0.26948</v>
+      </c>
+      <c r="L4" s="6">
+        <v>8.5882000000000005</v>
+      </c>
+      <c r="M4" s="4">
+        <v>178.47</v>
+      </c>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>288.16000000000003</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9.7515000000000004E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2599.9</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3789.1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>53.046999999999997</v>
+      </c>
+      <c r="H5" s="4">
+        <v>10.141</v>
+      </c>
+      <c r="I5" s="4">
+        <v>14.268000000000001</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1293.9000000000001</v>
+      </c>
+      <c r="K5" s="4">
+        <v>-0.27987000000000001</v>
+      </c>
+      <c r="L5" s="6">
+        <v>8.6928999999999998</v>
+      </c>
+      <c r="M5" s="4">
+        <v>180.95</v>
+      </c>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>293.16000000000003</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9.9207000000000004E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2650.6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3860.5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>53.222000000000001</v>
+      </c>
+      <c r="H6" s="4">
+        <v>10.161</v>
+      </c>
+      <c r="I6" s="4">
+        <v>14.288</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1304.7</v>
+      </c>
+      <c r="K6" s="4">
+        <v>-0.28983999999999999</v>
+      </c>
+      <c r="L6" s="6">
+        <v>8.7970000000000006</v>
+      </c>
+      <c r="M6" s="4">
+        <v>183.39</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>298.16000000000003</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.1009</v>
+      </c>
+      <c r="C7" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2701.5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3931.9</v>
+      </c>
+      <c r="G7" s="4">
+        <v>53.393999999999998</v>
+      </c>
+      <c r="H7" s="4">
+        <v>10.18</v>
+      </c>
+      <c r="I7" s="4">
+        <v>14.305999999999999</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1315.4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>-0.29942000000000002</v>
+      </c>
+      <c r="L7" s="6">
+        <v>8.900500000000001</v>
+      </c>
+      <c r="M7" s="4">
+        <v>185.81</v>
+      </c>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>303.16000000000003</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.10259</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2752.4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4003.5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>53.563000000000002</v>
+      </c>
+      <c r="H8" s="4">
+        <v>10.196999999999999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>14.324</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1326.1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>-0.30862000000000001</v>
+      </c>
+      <c r="L8" s="6">
+        <v>9.0034999999999989</v>
+      </c>
+      <c r="M8" s="4">
+        <v>188.20999999999998</v>
+      </c>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>308.16000000000003</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.10428</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2803.4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4075.2</v>
+      </c>
+      <c r="G9" s="4">
+        <v>53.73</v>
+      </c>
+      <c r="H9" s="4">
+        <v>10.212999999999999</v>
+      </c>
+      <c r="I9" s="4">
+        <v>14.339</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1336.7</v>
+      </c>
+      <c r="K9" s="4">
+        <v>-0.31747999999999998</v>
+      </c>
+      <c r="L9" s="6">
+        <v>9.1059999999999999</v>
+      </c>
+      <c r="M9" s="4">
+        <v>190.59</v>
+      </c>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>313.16000000000003</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.10598</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2854.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4146.8999999999996</v>
+      </c>
+      <c r="G10" s="4">
+        <v>53.895000000000003</v>
+      </c>
+      <c r="H10" s="4">
+        <v>10.228</v>
+      </c>
+      <c r="I10" s="4">
+        <v>14.353999999999999</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1347.2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>-0.32601000000000002</v>
+      </c>
+      <c r="L10" s="6">
+        <v>9.2080000000000002</v>
+      </c>
+      <c r="M10" s="4">
+        <v>192.95000000000002</v>
+      </c>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>318.16000000000003</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.10767</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2905.7</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4218.7</v>
+      </c>
+      <c r="G11" s="4">
+        <v>54.057000000000002</v>
+      </c>
+      <c r="H11" s="4">
+        <v>10.241</v>
+      </c>
+      <c r="I11" s="4">
+        <v>14.367000000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1357.6</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-0.33422000000000002</v>
+      </c>
+      <c r="L11" s="6">
+        <v>9.3094000000000001</v>
+      </c>
+      <c r="M11" s="4">
+        <v>195.28</v>
+      </c>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>323.16000000000003</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.10936</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2956.9</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4290.6000000000004</v>
+      </c>
+      <c r="G12" s="4">
+        <v>54.216999999999999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>10.254</v>
+      </c>
+      <c r="I12" s="4">
+        <v>14.38</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1368</v>
+      </c>
+      <c r="K12" s="4">
+        <v>-0.34214</v>
+      </c>
+      <c r="L12" s="6">
+        <v>9.410400000000001</v>
+      </c>
+      <c r="M12" s="4">
+        <v>197.58999999999997</v>
+      </c>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>328.16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.11105</v>
+      </c>
+      <c r="C13" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3008.2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4362.6000000000004</v>
+      </c>
+      <c r="G13" s="4">
+        <v>54.374000000000002</v>
+      </c>
+      <c r="H13" s="4">
+        <v>10.265000000000001</v>
+      </c>
+      <c r="I13" s="4">
+        <v>14.391</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1378.4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-0.34977999999999998</v>
+      </c>
+      <c r="L13" s="6">
+        <v>9.5109000000000012</v>
+      </c>
+      <c r="M13" s="4">
+        <v>199.89000000000001</v>
+      </c>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>333.16</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.11275</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3059.6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4434.5</v>
+      </c>
+      <c r="G14" s="4">
+        <v>54.529000000000003</v>
+      </c>
+      <c r="H14" s="4">
+        <v>10.276</v>
+      </c>
+      <c r="I14" s="4">
+        <v>14.401999999999999</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1388.6</v>
+      </c>
+      <c r="K14" s="4">
+        <v>-0.35715000000000002</v>
+      </c>
+      <c r="L14" s="6">
+        <v>9.6110000000000007</v>
+      </c>
+      <c r="M14" s="4">
+        <v>202.17</v>
+      </c>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>338.16</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.11444</v>
+      </c>
+      <c r="C15" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3111</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4506.6000000000004</v>
+      </c>
+      <c r="G15" s="4">
+        <v>54.682000000000002</v>
+      </c>
+      <c r="H15" s="4">
+        <v>10.285</v>
+      </c>
+      <c r="I15" s="4">
+        <v>14.411</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1398.8</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-0.36426999999999998</v>
+      </c>
+      <c r="L15" s="6">
+        <v>9.7105999999999995</v>
+      </c>
+      <c r="M15" s="4">
+        <v>204.43</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>343.16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.11613</v>
+      </c>
+      <c r="C16" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3162.4</v>
+      </c>
+      <c r="F16" s="4">
+        <v>4578.7</v>
+      </c>
+      <c r="G16" s="4">
+        <v>54.834000000000003</v>
+      </c>
+      <c r="H16" s="4">
+        <v>10.294</v>
+      </c>
+      <c r="I16" s="4">
+        <v>14.42</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1408.9</v>
+      </c>
+      <c r="K16" s="4">
+        <v>-0.37114999999999998</v>
+      </c>
+      <c r="L16" s="6">
+        <v>9.8096999999999994</v>
+      </c>
+      <c r="M16" s="4">
+        <v>206.67</v>
+      </c>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>348.16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.11781999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3213.9</v>
+      </c>
+      <c r="F17" s="4">
+        <v>4650.8</v>
+      </c>
+      <c r="G17" s="4">
+        <v>54.981999999999999</v>
+      </c>
+      <c r="H17" s="4">
+        <v>10.302</v>
+      </c>
+      <c r="I17" s="4">
+        <v>14.428000000000001</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1419</v>
+      </c>
+      <c r="K17" s="4">
+        <v>-0.37780000000000002</v>
+      </c>
+      <c r="L17" s="6">
+        <v>9.9085000000000001</v>
+      </c>
+      <c r="M17" s="4">
+        <v>208.89</v>
+      </c>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>353.16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.11952</v>
+      </c>
+      <c r="C18" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3265.5</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4723</v>
+      </c>
+      <c r="G18" s="4">
+        <v>55.128999999999998</v>
+      </c>
+      <c r="H18" s="4">
+        <v>10.31</v>
+      </c>
+      <c r="I18" s="4">
+        <v>14.435</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1429</v>
+      </c>
+      <c r="K18" s="4">
+        <v>-0.38423000000000002</v>
+      </c>
+      <c r="L18" s="6">
+        <v>10.007</v>
+      </c>
+      <c r="M18" s="4">
+        <v>211.10000000000002</v>
+      </c>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>358.16</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.12121</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3317</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4795.2</v>
+      </c>
+      <c r="G19" s="4">
+        <v>55.274000000000001</v>
+      </c>
+      <c r="H19" s="4">
+        <v>10.316000000000001</v>
+      </c>
+      <c r="I19" s="4">
+        <v>14.442</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1439</v>
+      </c>
+      <c r="K19" s="4">
+        <v>-0.39045000000000002</v>
+      </c>
+      <c r="L19" s="6">
+        <v>10.105</v>
+      </c>
+      <c r="M19" s="4">
+        <v>213.29999999999998</v>
+      </c>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>363.16</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.1229</v>
+      </c>
+      <c r="C20" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3368.6</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4867.3999999999996</v>
+      </c>
+      <c r="G20" s="4">
+        <v>55.417000000000002</v>
+      </c>
+      <c r="H20" s="4">
+        <v>10.323</v>
+      </c>
+      <c r="I20" s="4">
+        <v>14.448</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1448.9</v>
+      </c>
+      <c r="K20" s="4">
+        <v>-0.39648</v>
+      </c>
+      <c r="L20" s="6">
+        <v>10.202</v>
+      </c>
+      <c r="M20" s="4">
+        <v>215.48000000000002</v>
+      </c>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>368.16</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.12459000000000001</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3420.3</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4939.7</v>
+      </c>
+      <c r="G21" s="4">
+        <v>55.558999999999997</v>
+      </c>
+      <c r="H21" s="4">
+        <v>10.327999999999999</v>
+      </c>
+      <c r="I21" s="4">
+        <v>14.454000000000001</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1458.7</v>
+      </c>
+      <c r="K21" s="4">
+        <v>-0.40231</v>
+      </c>
+      <c r="L21" s="6">
+        <v>10.299000000000001</v>
+      </c>
+      <c r="M21" s="4">
+        <v>217.64</v>
+      </c>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>373.16</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.12629000000000001</v>
+      </c>
+      <c r="C22" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3471.9</v>
+      </c>
+      <c r="F22" s="4">
+        <v>5012</v>
+      </c>
+      <c r="G22" s="4">
+        <v>55.698</v>
+      </c>
+      <c r="H22" s="4">
+        <v>10.333</v>
+      </c>
+      <c r="I22" s="4">
+        <v>14.459</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1468.4</v>
+      </c>
+      <c r="K22" s="4">
+        <v>-0.40795999999999999</v>
+      </c>
+      <c r="L22" s="6">
+        <v>10.396000000000001</v>
+      </c>
+      <c r="M22" s="4">
+        <v>219.79999999999998</v>
+      </c>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>378.16</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.12798000000000001</v>
+      </c>
+      <c r="C23" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D23" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E23" s="4">
+        <v>3523.6</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5084.3</v>
+      </c>
+      <c r="G23" s="4">
+        <v>55.835999999999999</v>
+      </c>
+      <c r="H23" s="4">
+        <v>10.337999999999999</v>
+      </c>
+      <c r="I23" s="4">
+        <v>14.464</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1478.2</v>
+      </c>
+      <c r="K23" s="4">
+        <v>-0.41343999999999997</v>
+      </c>
+      <c r="L23" s="6">
+        <v>10.492000000000001</v>
+      </c>
+      <c r="M23" s="4">
+        <v>221.92999999999998</v>
+      </c>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>383.16</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.12967000000000001</v>
+      </c>
+      <c r="C24" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3575.3</v>
+      </c>
+      <c r="F24" s="4">
+        <v>5156.6000000000004</v>
+      </c>
+      <c r="G24" s="4">
+        <v>55.970999999999997</v>
+      </c>
+      <c r="H24" s="4">
+        <v>10.342000000000001</v>
+      </c>
+      <c r="I24" s="4">
+        <v>14.468</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1487.8</v>
+      </c>
+      <c r="K24" s="4">
+        <v>-0.41874</v>
+      </c>
+      <c r="L24" s="6">
+        <v>10.587999999999999</v>
+      </c>
+      <c r="M24" s="4">
+        <v>224.06</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>388.16</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.13136</v>
+      </c>
+      <c r="C25" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D25" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3627</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5229</v>
+      </c>
+      <c r="G25" s="4">
+        <v>56.106000000000002</v>
+      </c>
+      <c r="H25" s="4">
+        <v>10.346</v>
+      </c>
+      <c r="I25" s="4">
+        <v>14.472</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1497.4</v>
+      </c>
+      <c r="K25" s="4">
+        <v>-0.42388999999999999</v>
+      </c>
+      <c r="L25" s="6">
+        <v>10.683999999999999</v>
+      </c>
+      <c r="M25" s="4">
+        <v>226.17000000000002</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>393.16</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.13306000000000001</v>
+      </c>
+      <c r="C26" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E26" s="4">
+        <v>3678.7</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5301.4</v>
+      </c>
+      <c r="G26" s="4">
+        <v>56.238</v>
+      </c>
+      <c r="H26" s="4">
+        <v>10.35</v>
+      </c>
+      <c r="I26" s="4">
+        <v>14.475</v>
+      </c>
+      <c r="J26" s="4">
+        <v>1506.9</v>
+      </c>
+      <c r="K26" s="4">
+        <v>-0.42887999999999998</v>
+      </c>
+      <c r="L26" s="6">
+        <v>10.779</v>
+      </c>
+      <c r="M26" s="4">
+        <v>228.28</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>398.16</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.13475000000000001</v>
+      </c>
+      <c r="C27" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D27" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3730.5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5373.8</v>
+      </c>
+      <c r="G27" s="4">
+        <v>56.369</v>
+      </c>
+      <c r="H27" s="4">
+        <v>10.353</v>
+      </c>
+      <c r="I27" s="4">
+        <v>14.478999999999999</v>
+      </c>
+      <c r="J27" s="4">
+        <v>1516.4</v>
+      </c>
+      <c r="K27" s="4">
+        <v>-0.43371999999999999</v>
+      </c>
+      <c r="L27" s="6">
+        <v>10.873999999999999</v>
+      </c>
+      <c r="M27" s="4">
+        <v>230.37</v>
+      </c>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>403.16</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.13644000000000001</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3782.3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>5446.2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>56.497999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>10.356</v>
+      </c>
+      <c r="I28" s="4">
+        <v>14.481999999999999</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1525.9</v>
+      </c>
+      <c r="K28" s="4">
+        <v>-0.43841999999999998</v>
+      </c>
+      <c r="L28" s="6">
+        <v>10.968</v>
+      </c>
+      <c r="M28" s="4">
+        <v>232.45</v>
+      </c>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>408.16</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.13813</v>
+      </c>
+      <c r="C29" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3834.1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>5518.6</v>
+      </c>
+      <c r="G29" s="4">
+        <v>56.625999999999998</v>
+      </c>
+      <c r="H29" s="4">
+        <v>10.359</v>
+      </c>
+      <c r="I29" s="4">
+        <v>14.484</v>
+      </c>
+      <c r="J29" s="4">
+        <v>1535.2</v>
+      </c>
+      <c r="K29" s="4">
+        <v>-0.44297999999999998</v>
+      </c>
+      <c r="L29" s="6">
+        <v>11.063000000000001</v>
+      </c>
+      <c r="M29" s="4">
+        <v>234.52</v>
+      </c>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>413.16</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.13982</v>
+      </c>
+      <c r="C30" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D30" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3885.9</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5591</v>
+      </c>
+      <c r="G30" s="4">
+        <v>56.752000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>10.361000000000001</v>
+      </c>
+      <c r="I30" s="4">
+        <v>14.487</v>
+      </c>
+      <c r="J30" s="4">
+        <v>1544.6</v>
+      </c>
+      <c r="K30" s="4">
+        <v>-0.44740999999999997</v>
+      </c>
+      <c r="L30" s="6">
+        <v>11.155999999999999</v>
+      </c>
+      <c r="M30" s="4">
+        <v>236.58</v>
+      </c>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>418.16</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.14152000000000001</v>
+      </c>
+      <c r="C31" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3937.7</v>
+      </c>
+      <c r="F31" s="4">
+        <v>5663.5</v>
+      </c>
+      <c r="G31" s="4">
+        <v>56.875999999999998</v>
+      </c>
+      <c r="H31" s="4">
+        <v>10.364000000000001</v>
+      </c>
+      <c r="I31" s="4">
+        <v>14.489000000000001</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1553.8</v>
+      </c>
+      <c r="K31" s="4">
+        <v>-0.45171</v>
+      </c>
+      <c r="L31" s="6">
+        <v>11.25</v>
+      </c>
+      <c r="M31" s="4">
+        <v>238.63</v>
+      </c>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>423.16</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.14321</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>12.195</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3989.5</v>
+      </c>
+      <c r="F32" s="4">
+        <v>5736</v>
+      </c>
+      <c r="G32" s="4">
+        <v>57</v>
+      </c>
+      <c r="H32" s="4">
+        <v>10.366</v>
+      </c>
+      <c r="I32" s="4">
+        <v>14.491</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1563</v>
+      </c>
+      <c r="K32" s="4">
+        <v>-0.45589000000000002</v>
+      </c>
+      <c r="L32" s="6">
+        <v>11.343</v>
+      </c>
+      <c r="M32" s="4">
+        <v>240.67</v>
+      </c>
+      <c r="O32" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23CE22A-8B52-4E0E-9B7A-5878CC3A4604}">
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>273.16000000000003</v>
+      </c>
+      <c r="B2" s="4">
         <v>9.2896000000000006E-2</v>
       </c>
       <c r="C2" s="4">
@@ -2878,14 +2927,15 @@
       <c r="K2" s="4">
         <v>3.1722999999999999</v>
       </c>
-      <c r="L2" s="5">
-        <v>1.9142000000000001E-5</v>
+      <c r="L2" s="6">
+        <v>19.141999999999999</v>
       </c>
       <c r="M2" s="4">
-        <v>2.4346E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24.346</v>
+      </c>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>278.16000000000003</v>
       </c>
@@ -2919,14 +2969,15 @@
       <c r="K3" s="4">
         <v>3.0665</v>
       </c>
-      <c r="L3" s="5">
-        <v>1.9428000000000001E-5</v>
+      <c r="L3" s="6">
+        <v>19.428000000000001</v>
       </c>
       <c r="M3" s="4">
-        <v>2.4749E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24.748999999999999</v>
+      </c>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>283.16000000000003</v>
       </c>
@@ -2960,14 +3011,15 @@
       <c r="K4" s="4">
         <v>2.9651000000000001</v>
       </c>
-      <c r="L4" s="5">
-        <v>1.9711000000000002E-5</v>
+      <c r="L4" s="6">
+        <v>19.711000000000002</v>
       </c>
       <c r="M4" s="4">
-        <v>2.5149999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25.15</v>
+      </c>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>288.16000000000003</v>
       </c>
@@ -3001,14 +3053,15 @@
       <c r="K5" s="4">
         <v>2.8679000000000001</v>
       </c>
-      <c r="L5" s="5">
-        <v>1.9993E-5</v>
+      <c r="L5" s="6">
+        <v>19.992999999999999</v>
       </c>
       <c r="M5" s="4">
-        <v>2.5548999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25.548999999999999</v>
+      </c>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>293.16000000000003</v>
       </c>
@@ -3042,14 +3095,15 @@
       <c r="K6" s="4">
         <v>2.7746</v>
       </c>
-      <c r="L6" s="5">
-        <v>2.0273000000000001E-5</v>
+      <c r="L6" s="6">
+        <v>20.273</v>
       </c>
       <c r="M6" s="4">
-        <v>2.5946E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25.946000000000002</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>298.16000000000003</v>
       </c>
@@ -3083,14 +3137,15 @@
       <c r="K7" s="4">
         <v>2.6850000000000001</v>
       </c>
-      <c r="L7" s="5">
-        <v>2.0551E-5</v>
+      <c r="L7" s="6">
+        <v>20.551000000000002</v>
       </c>
       <c r="M7" s="4">
-        <v>2.6341E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26.341000000000001</v>
+      </c>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>303.16000000000003</v>
       </c>
@@ -3124,14 +3179,15 @@
       <c r="K8" s="4">
         <v>2.5989</v>
       </c>
-      <c r="L8" s="5">
-        <v>2.0826999999999999E-5</v>
+      <c r="L8" s="6">
+        <v>20.826999999999998</v>
       </c>
       <c r="M8" s="4">
-        <v>2.6734999999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26.734999999999999</v>
+      </c>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>308.16000000000003</v>
       </c>
@@ -3165,14 +3221,15 @@
       <c r="K9" s="4">
         <v>2.5160999999999998</v>
       </c>
-      <c r="L9" s="5">
-        <v>2.1101E-5</v>
+      <c r="L9" s="6">
+        <v>21.100999999999999</v>
       </c>
       <c r="M9" s="4">
-        <v>2.7126999999999998E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27.126999999999999</v>
+      </c>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>313.16000000000003</v>
       </c>
@@ -3206,14 +3263,15 @@
       <c r="K10" s="4">
         <v>2.4363999999999999</v>
       </c>
-      <c r="L10" s="5">
-        <v>2.1373E-5</v>
+      <c r="L10" s="6">
+        <v>21.373000000000001</v>
       </c>
       <c r="M10" s="4">
-        <v>2.7517E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27.516999999999999</v>
+      </c>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>318.16000000000003</v>
       </c>
@@ -3247,14 +3305,15 @@
       <c r="K11" s="4">
         <v>2.3597000000000001</v>
       </c>
-      <c r="L11" s="5">
-        <v>2.1644000000000001E-5</v>
+      <c r="L11" s="6">
+        <v>21.644000000000002</v>
       </c>
       <c r="M11" s="4">
-        <v>2.7904999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27.904999999999998</v>
+      </c>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>323.16000000000003</v>
       </c>
@@ -3288,14 +3347,15 @@
       <c r="K12" s="4">
         <v>2.2856999999999998</v>
       </c>
-      <c r="L12" s="5">
-        <v>2.1912999999999998E-5</v>
+      <c r="L12" s="6">
+        <v>21.912999999999997</v>
       </c>
       <c r="M12" s="4">
-        <v>2.8292000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>28.292000000000002</v>
+      </c>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>328.16</v>
       </c>
@@ -3329,14 +3389,15 @@
       <c r="K13" s="4">
         <v>2.2143999999999999</v>
       </c>
-      <c r="L13" s="5">
-        <v>2.2180000000000001E-5</v>
+      <c r="L13" s="6">
+        <v>22.18</v>
       </c>
       <c r="M13" s="4">
-        <v>2.8677000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>28.677</v>
+      </c>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>333.16</v>
       </c>
@@ -3370,14 +3431,15 @@
       <c r="K14" s="4">
         <v>2.1456</v>
       </c>
-      <c r="L14" s="5">
-        <v>2.2446000000000002E-5</v>
+      <c r="L14" s="6">
+        <v>22.446000000000002</v>
       </c>
       <c r="M14" s="4">
-        <v>2.9059999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29.06</v>
+      </c>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>338.16</v>
       </c>
@@ -3411,14 +3473,15 @@
       <c r="K15" s="4">
         <v>2.0792000000000002</v>
       </c>
-      <c r="L15" s="5">
-        <v>2.2710000000000001E-5</v>
+      <c r="L15" s="6">
+        <v>22.71</v>
       </c>
       <c r="M15" s="4">
-        <v>2.9441999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29.442</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>343.16</v>
       </c>
@@ -3452,14 +3515,15 @@
       <c r="K16" s="4">
         <v>2.0150999999999999</v>
       </c>
-      <c r="L16" s="5">
-        <v>2.2972E-5</v>
+      <c r="L16" s="6">
+        <v>22.972000000000001</v>
       </c>
       <c r="M16" s="4">
-        <v>2.9822000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29.822000000000003</v>
+      </c>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>348.16</v>
       </c>
@@ -3493,14 +3557,15 @@
       <c r="K17" s="4">
         <v>1.9532</v>
       </c>
-      <c r="L17" s="5">
-        <v>2.3232000000000001E-5</v>
+      <c r="L17" s="6">
+        <v>23.231999999999999</v>
       </c>
       <c r="M17" s="4">
-        <v>3.0200999999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30.200999999999997</v>
+      </c>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>353.16</v>
       </c>
@@ -3534,14 +3599,15 @@
       <c r="K18" s="4">
         <v>1.8933</v>
       </c>
-      <c r="L18" s="5">
-        <v>2.3490999999999999E-5</v>
+      <c r="L18" s="6">
+        <v>23.491</v>
       </c>
       <c r="M18" s="4">
-        <v>3.0578000000000001E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30.577999999999999</v>
+      </c>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>358.16</v>
       </c>
@@ -3575,14 +3641,15 @@
       <c r="K19" s="4">
         <v>1.8353999999999999</v>
       </c>
-      <c r="L19" s="5">
-        <v>2.3748999999999999E-5</v>
+      <c r="L19" s="6">
+        <v>23.748999999999999</v>
       </c>
       <c r="M19" s="4">
-        <v>3.0953000000000001E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30.953000000000003</v>
+      </c>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>363.16</v>
       </c>
@@ -3616,14 +3683,15 @@
       <c r="K20" s="4">
         <v>1.7794000000000001</v>
       </c>
-      <c r="L20" s="5">
-        <v>2.4005000000000001E-5</v>
+      <c r="L20" s="6">
+        <v>24.005000000000003</v>
       </c>
       <c r="M20" s="4">
-        <v>3.1327000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>368.16</v>
       </c>
@@ -3657,14 +3725,15 @@
       <c r="K21" s="4">
         <v>1.7252000000000001</v>
       </c>
-      <c r="L21" s="5">
-        <v>2.4258999999999999E-5</v>
+      <c r="L21" s="6">
+        <v>24.259</v>
       </c>
       <c r="M21" s="4">
-        <v>3.1699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31.7</v>
+      </c>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>373.16</v>
       </c>
@@ -3698,14 +3767,15 @@
       <c r="K22" s="4">
         <v>1.6727000000000001</v>
       </c>
-      <c r="L22" s="5">
-        <v>2.4511999999999998E-5</v>
+      <c r="L22" s="6">
+        <v>24.511999999999997</v>
       </c>
       <c r="M22" s="4">
-        <v>3.2071000000000002E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32.071000000000005</v>
+      </c>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>378.16</v>
       </c>
@@ -3739,14 +3809,15 @@
       <c r="K23" s="4">
         <v>1.6218999999999999</v>
       </c>
-      <c r="L23" s="5">
-        <v>2.4763999999999999E-5</v>
+      <c r="L23" s="6">
+        <v>24.763999999999999</v>
       </c>
       <c r="M23" s="4">
-        <v>3.2440999999999998E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32.440999999999995</v>
+      </c>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>383.16</v>
       </c>
@@ -3780,14 +3851,15 @@
       <c r="K24" s="4">
         <v>1.5727</v>
       </c>
-      <c r="L24" s="5">
-        <v>2.5014000000000001E-5</v>
+      <c r="L24" s="6">
+        <v>25.014000000000003</v>
       </c>
       <c r="M24" s="4">
-        <v>3.2809999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32.81</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>388.16</v>
       </c>
@@ -3821,14 +3893,15 @@
       <c r="K25" s="4">
         <v>1.5248999999999999</v>
       </c>
-      <c r="L25" s="5">
-        <v>2.5262999999999999E-5</v>
+      <c r="L25" s="6">
+        <v>25.262999999999998</v>
       </c>
       <c r="M25" s="4">
-        <v>3.3176999999999998E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33.177</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>393.16</v>
       </c>
@@ -3862,14 +3935,15 @@
       <c r="K26" s="4">
         <v>1.4786999999999999</v>
       </c>
-      <c r="L26" s="5">
-        <v>2.5510000000000001E-5</v>
+      <c r="L26" s="6">
+        <v>25.51</v>
       </c>
       <c r="M26" s="4">
-        <v>3.3542000000000002E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33.542000000000002</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>398.16</v>
       </c>
@@ -3903,14 +3977,15 @@
       <c r="K27" s="4">
         <v>1.4338</v>
       </c>
-      <c r="L27" s="5">
-        <v>2.5755999999999999E-5</v>
+      <c r="L27" s="6">
+        <v>25.756</v>
       </c>
       <c r="M27" s="4">
-        <v>3.3907E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33.906999999999996</v>
+      </c>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>403.16</v>
       </c>
@@ -3944,14 +4019,15 @@
       <c r="K28" s="4">
         <v>1.3903000000000001</v>
       </c>
-      <c r="L28" s="5">
-        <v>2.5999999999999998E-5</v>
+      <c r="L28" s="6">
+        <v>26</v>
       </c>
       <c r="M28" s="4">
-        <v>3.4270000000000002E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>408.16</v>
       </c>
@@ -3985,14 +4061,15 @@
       <c r="K29" s="4">
         <v>1.3481000000000001</v>
       </c>
-      <c r="L29" s="5">
-        <v>2.6244000000000001E-5</v>
+      <c r="L29" s="6">
+        <v>26.244</v>
       </c>
       <c r="M29" s="4">
-        <v>3.4631000000000002E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34.631</v>
+      </c>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>413.16</v>
       </c>
@@ -4026,14 +4103,15 @@
       <c r="K30" s="4">
         <v>1.3070999999999999</v>
       </c>
-      <c r="L30" s="5">
-        <v>2.6486E-5</v>
+      <c r="L30" s="6">
+        <v>26.486000000000001</v>
       </c>
       <c r="M30" s="4">
-        <v>3.4992000000000002E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34.992000000000004</v>
+      </c>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>418.16</v>
       </c>
@@ -4067,14 +4145,15 @@
       <c r="K31" s="4">
         <v>1.2673000000000001</v>
       </c>
-      <c r="L31" s="5">
-        <v>2.6726000000000001E-5</v>
+      <c r="L31" s="6">
+        <v>26.726000000000003</v>
       </c>
       <c r="M31" s="4">
-        <v>3.5351E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>35.350999999999999</v>
+      </c>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>423.16</v>
       </c>
@@ -4108,12 +4187,13 @@
       <c r="K32" s="4">
         <v>1.2285999999999999</v>
       </c>
-      <c r="L32" s="5">
-        <v>2.6965999999999999E-5</v>
+      <c r="L32" s="6">
+        <v>26.965999999999998</v>
       </c>
       <c r="M32" s="4">
-        <v>3.5708999999999998E-2</v>
-      </c>
+        <v>35.708999999999996</v>
+      </c>
+      <c r="O32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>